<commit_message>
pyNMS with QT part 1
</commit_message>
<xml_diff>
--- a/Workspace/import_hostname.xlsx
+++ b/Workspace/import_hostname.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>second_device</t>
+  </si>
+  <si>
+    <t>router3</t>
+  </si>
+  <si>
+    <t>third_device</t>
   </si>
 </sst>
 </file>
@@ -354,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -389,6 +395,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
pyNMS QT part 92
</commit_message>
<xml_diff>
--- a/Workspace/import_hostname.xlsx
+++ b/Workspace/import_hostname.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="router" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>name</t>
   </si>
@@ -43,12 +43,24 @@
   </si>
   <si>
     <t>third_device</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>Cisco</t>
+  </si>
+  <si>
+    <t>Juniper</t>
+  </si>
+  <si>
+    <t>Nokia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -360,47 +372,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>